<commit_message>
add get users by project id
</commit_message>
<xml_diff>
--- a/ListIssueToEnhance.xlsx
+++ b/ListIssueToEnhance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\cnpmcs\Source_BE\ErrorMonitoring_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6EAF34-012F-45D1-B0E0-3AF5A4856418}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D691C3-B6EF-451C-990E-9E6BB088D86C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>STT</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>validate admin mới có quyền mời member mới</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>trạng thái</t>
   </si>
 </sst>
 </file>
@@ -381,18 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,8 +415,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -420,7 +433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -434,9 +447,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add search user/project extent method
</commit_message>
<xml_diff>
--- a/ListIssueToEnhance.xlsx
+++ b/ListIssueToEnhance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\cnpmcs\Source_BE\ErrorMonitoring_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D691C3-B6EF-451C-990E-9E6BB088D86C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49741790-B1F6-430C-87FF-2292644C190D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>STT</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>trạng thái</t>
+  </si>
+  <si>
+    <t>xóa project khi role admin</t>
+  </si>
+  <si>
+    <t>kiểm tra email có thật không</t>
+  </si>
+  <si>
+    <t>cao</t>
+  </si>
+  <si>
+    <t>tích hợp trello</t>
+  </si>
+  <si>
+    <t>đã thêm</t>
+  </si>
+  <si>
+    <t>chờ</t>
   </si>
 </sst>
 </file>
@@ -390,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +450,9 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -446,6 +467,9 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -459,6 +483,45 @@
       </c>
       <c r="D4" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create issue and filter
</commit_message>
<xml_diff>
--- a/ListIssueToEnhance.xlsx
+++ b/ListIssueToEnhance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\cnpmcs\Source_BE\ErrorMonitoring_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF5A4DD-70DB-474B-8B4F-C2DA375131CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDF008C-86CD-4E05-97F9-1DC598EA6594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>khi get users thì bỏ qua các project được asign nhưng bị active = false</t>
+  </si>
+  <si>
+    <t>thêm API update avatar</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +547,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>